<commit_message>
Unreported Branches analysis implemented
</commit_message>
<xml_diff>
--- a/Input Paths.xlsx
+++ b/Input Paths.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Variable Name</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>supplier_name</t>
-  </si>
-  <si>
-    <t>Humana (Right Source)</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -110,9 +107,6 @@
     <t>Name of File that contains factoring information of all NDC, staple file, only needs to be modified in case of new information</t>
   </si>
   <si>
-    <t>Humana (Right Source)_SEP23</t>
-  </si>
-  <si>
     <t>SAP Data OCT'23</t>
   </si>
   <si>
@@ -189,6 +183,21 @@
   </si>
   <si>
     <t>ndc_factoring_values_file</t>
+  </si>
+  <si>
+    <t>RELIANCERX</t>
+  </si>
+  <si>
+    <t>RELIANCERX_SEP23</t>
+  </si>
+  <si>
+    <t>RELIANCERX Ins</t>
+  </si>
+  <si>
+    <t>RELIANCERX BO</t>
+  </si>
+  <si>
+    <t>RELIANCERX BRANCH</t>
   </si>
 </sst>
 </file>
@@ -408,12 +417,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -450,6 +453,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -739,241 +748,247 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.21875" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="110.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>36</v>
+      <c r="A5" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+    <row r="7" spans="1:3" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="36"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="23"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>40</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>41</v>
+      <c r="A10" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>42</v>
+      <c r="A11" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>43</v>
+      <c r="A12" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
-        <v>44</v>
+      <c r="A13" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
-        <v>45</v>
+      <c r="A14" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>46</v>
+      <c r="A15" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
         <v>47</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
-        <v>49</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>50</v>
+      <c r="A19" s="32" t="s">
+        <v>48</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
+    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B22" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
+      <c r="C22" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B23" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
+      <c r="C23" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B24" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="21" t="s">
+      <c r="C24" s="21" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>